<commit_message>
Perform Agglomerative Clustering, choose optimal nr. clusters with elbow plot and generate dendogram. Modifiy DBSCAN so that the optimal solution found doesn't produce a majority of -1 cluster labels (i.e. noise class). Print out what percentage of the data was assigned to each cluster.
</commit_message>
<xml_diff>
--- a/Tables/Classification_Results.xlsx
+++ b/Tables/Classification_Results.xlsx
@@ -1,84 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HFO\Documents\MachineLearning\Capstone_Projects\ml_framework\Tables\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8739B65-EB99-46DC-B00D-E6B0AF78D93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>Precision</t>
-  </si>
-  <si>
-    <t>Recall</t>
-  </si>
-  <si>
-    <t>Accuracy</t>
-  </si>
-  <si>
-    <t>F1-Score</t>
-  </si>
-  <si>
-    <t>LogisticRegressionClassifier</t>
-  </si>
-  <si>
-    <t>KNN_Classifier</t>
-  </si>
-  <si>
-    <t>DecisionTreeClassifier</t>
-  </si>
-  <si>
-    <t>RandomForestClassifier</t>
-  </si>
-  <si>
-    <t>XGBoostClassifier</t>
-  </si>
-  <si>
-    <t>ANN_TF_Classifier</t>
-  </si>
-  <si>
-    <t>SupportVectorClassifier</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -93,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -417,174 +420,198 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Recall</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>F1-Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>LogisticRegressionClassifier</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.6360913806200214</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.5206927925356021</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.6514688166064313</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.541070036062836</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>KNN_Classifier</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.6844618002341644</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.6377725662793875</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.6863126679640441</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.6544319196936332</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>DecisionTreeClassifier</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.693998767585976</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.6459459439728221</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.7178204058938004</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.6557581910474266</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>RandomForestClassifier</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.8019559995330805</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.759291948294522</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.7798165137614679</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.7695516203726432</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>XGBoostClassifier</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.81949518273149</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.7933953779493348</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.8108609026040219</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.805071205414861</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>0.65496879694130405</v>
-      </c>
-      <c r="D2">
-        <v>0.53404950901325088</v>
-      </c>
-      <c r="E2">
-        <v>0.65777036419238255</v>
-      </c>
-      <c r="F2">
-        <v>0.55306362786639085</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ANN_TF_Classifier</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.8060755855954959</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.7774825382728457</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.8002965434158095</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.790335976241099</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>0.68061090720926443</v>
-      </c>
-      <c r="D3">
-        <v>0.60311842811137917</v>
-      </c>
-      <c r="E3">
-        <v>0.68112315818737834</v>
-      </c>
-      <c r="F3">
-        <v>0.62473901428027245</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>0.67335976857165292</v>
-      </c>
-      <c r="D4">
-        <v>0.62144875091739027</v>
-      </c>
-      <c r="E4">
-        <v>0.70855342414975442</v>
-      </c>
-      <c r="F4">
-        <v>0.63157943750709966</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>0.79896014156905282</v>
-      </c>
-      <c r="D5">
-        <v>0.75560379346019158</v>
-      </c>
-      <c r="E5">
-        <v>0.77666573996849231</v>
-      </c>
-      <c r="F5">
-        <v>0.76767358645242223</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>0.82033408787121131</v>
-      </c>
-      <c r="D6">
-        <v>0.78603383529984427</v>
-      </c>
-      <c r="E6">
-        <v>0.80696877027152258</v>
-      </c>
-      <c r="F6">
-        <v>0.80167249185896117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>0.79703379500755656</v>
-      </c>
-      <c r="D7">
-        <v>0.76106981613737135</v>
-      </c>
-      <c r="E7">
-        <v>0.78871281623575207</v>
-      </c>
-      <c r="F7">
-        <v>0.7748539244330428</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8">
-        <v>0.7901899218388756</v>
-      </c>
-      <c r="D8">
-        <v>0.74426769654024338</v>
-      </c>
-      <c r="E8">
-        <v>0.77805578723009916</v>
-      </c>
-      <c r="F8">
-        <v>0.76429504395420422</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SupportVectorClassifier</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.7826117515007261</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.7474896052132372</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.7807432119358725</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.7628955906282211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct corner case where no input data is provided for the classifiers or regressors. Save all models either as pickle files, keras or xgboost format. Save data analyzers for classification and regression.
</commit_message>
<xml_diff>
--- a/Tables/Classification_Results.xlsx
+++ b/Tables/Classification_Results.xlsx
@@ -470,16 +470,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.6360913806200214</v>
+        <v>0.6495703901946965</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5206927925356021</v>
+        <v>0.5336804966524851</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6514688166064313</v>
+        <v>0.6598091001760726</v>
       </c>
       <c r="F2" t="n">
-        <v>0.541070036062836</v>
+        <v>0.5550511827678311</v>
       </c>
     </row>
     <row r="3">
@@ -492,16 +492,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.6844618002341644</v>
+        <v>0.6747805441581174</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6377725662793875</v>
+        <v>0.6277410221681932</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6863126679640441</v>
+        <v>0.6805671392827356</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6544319196936332</v>
+        <v>0.6452157957942443</v>
       </c>
     </row>
     <row r="4">
@@ -514,16 +514,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.693998767585976</v>
+        <v>0.7085126875091203</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6459459439728221</v>
+        <v>0.6145867026921692</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7178204058938004</v>
+        <v>0.7127235659345751</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6557581910474266</v>
+        <v>0.6385898432540839</v>
       </c>
     </row>
     <row r="5">
@@ -536,16 +536,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.8019559995330805</v>
+        <v>0.7977292576506659</v>
       </c>
       <c r="D5" t="n">
-        <v>0.759291948294522</v>
+        <v>0.7590446704583426</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7798165137614679</v>
+        <v>0.7795385043091465</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7695516203726432</v>
+        <v>0.7687835241052147</v>
       </c>
     </row>
     <row r="6">
@@ -558,16 +558,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.81949518273149</v>
+        <v>0.8133977704366796</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7933953779493348</v>
+        <v>0.7876622016340096</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8108609026040219</v>
+        <v>0.8059494022796775</v>
       </c>
       <c r="F6" t="n">
-        <v>0.805071205414861</v>
+        <v>0.7992097196385826</v>
       </c>
     </row>
     <row r="7">
@@ -580,16 +580,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.8060755855954959</v>
+        <v>0.8045213424983151</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7774825382728457</v>
+        <v>0.7636442298603677</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8002965434158095</v>
+        <v>0.7972384394402743</v>
       </c>
       <c r="F7" t="n">
-        <v>0.790335976241099</v>
+        <v>0.7817481003397651</v>
       </c>
     </row>
     <row r="8">
@@ -602,16 +602,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.7826117515007261</v>
+        <v>0.7717053046795664</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7474896052132372</v>
+        <v>0.7320382797320696</v>
       </c>
       <c r="E8" t="n">
-        <v>0.7807432119358725</v>
+        <v>0.7740709850801594</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7628955906282211</v>
+        <v>0.7494307527014981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merge with working commit
</commit_message>
<xml_diff>
--- a/Tables/Classification_Results.xlsx
+++ b/Tables/Classification_Results.xlsx
@@ -470,16 +470,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.6495703901946965</v>
+        <v>0.6475450443515565</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5336804966524851</v>
+        <v>0.5304488830553094</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6598091001760726</v>
+        <v>0.6562876471133352</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5550511827678311</v>
+        <v>0.5531300020617894</v>
       </c>
     </row>
     <row r="3">
@@ -492,16 +492,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.6747805441581174</v>
+        <v>0.6788555333890164</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6277410221681932</v>
+        <v>0.6330308881811546</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6805671392827356</v>
+        <v>0.6844592716152349</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6452157957942443</v>
+        <v>0.6495117009622303</v>
       </c>
     </row>
     <row r="4">
@@ -514,16 +514,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.7085126875091203</v>
+        <v>0.6978232450277249</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6145867026921692</v>
+        <v>0.6613670820266967</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7127235659345751</v>
+        <v>0.7167083680845149</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6385898432540839</v>
+        <v>0.6607971017287977</v>
       </c>
     </row>
     <row r="5">
@@ -536,16 +536,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.7977292576506659</v>
+        <v>0.8060669117162877</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7590446704583426</v>
+        <v>0.7715082882922708</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7795385043091465</v>
+        <v>0.7843573348160504</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7687835241052147</v>
+        <v>0.7794834848664745</v>
       </c>
     </row>
     <row r="6">
@@ -558,16 +558,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.8133977704366796</v>
+        <v>0.8219834940351166</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7876622016340096</v>
+        <v>0.8018011998335816</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8059494022796775</v>
+        <v>0.8102122138819386</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7992097196385826</v>
+        <v>0.8106492623521262</v>
       </c>
     </row>
     <row r="7">
@@ -580,16 +580,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.8045213424983151</v>
+        <v>0.7957164589409468</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7636442298603677</v>
+        <v>0.7804162539177379</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7972384394402743</v>
+        <v>0.7969604299879529</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7817481003397651</v>
+        <v>0.7872969362904352</v>
       </c>
     </row>
     <row r="8">
@@ -602,16 +602,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.7717053046795664</v>
+        <v>0.7879161065596556</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7320382797320696</v>
+        <v>0.7512293710654735</v>
       </c>
       <c r="E8" t="n">
-        <v>0.7740709850801594</v>
+        <v>0.7833379668242053</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7494307527014981</v>
+        <v>0.7670381257688823</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "merge with working commit"
This reverts commit 6289c2263c586faa56d11395da5506445c1b558a.
</commit_message>
<xml_diff>
--- a/Tables/Classification_Results.xlsx
+++ b/Tables/Classification_Results.xlsx
@@ -470,16 +470,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.6475450443515565</v>
+        <v>0.6495703901946965</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5304488830553094</v>
+        <v>0.5336804966524851</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6562876471133352</v>
+        <v>0.6598091001760726</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5531300020617894</v>
+        <v>0.5550511827678311</v>
       </c>
     </row>
     <row r="3">
@@ -492,16 +492,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.6788555333890164</v>
+        <v>0.6747805441581174</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6330308881811546</v>
+        <v>0.6277410221681932</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6844592716152349</v>
+        <v>0.6805671392827356</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6495117009622303</v>
+        <v>0.6452157957942443</v>
       </c>
     </row>
     <row r="4">
@@ -514,16 +514,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.6978232450277249</v>
+        <v>0.7085126875091203</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6613670820266967</v>
+        <v>0.6145867026921692</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7167083680845149</v>
+        <v>0.7127235659345751</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6607971017287977</v>
+        <v>0.6385898432540839</v>
       </c>
     </row>
     <row r="5">
@@ -536,16 +536,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.8060669117162877</v>
+        <v>0.7977292576506659</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7715082882922708</v>
+        <v>0.7590446704583426</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7843573348160504</v>
+        <v>0.7795385043091465</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7794834848664745</v>
+        <v>0.7687835241052147</v>
       </c>
     </row>
     <row r="6">
@@ -558,16 +558,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.8219834940351166</v>
+        <v>0.8133977704366796</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8018011998335816</v>
+        <v>0.7876622016340096</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8102122138819386</v>
+        <v>0.8059494022796775</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8106492623521262</v>
+        <v>0.7992097196385826</v>
       </c>
     </row>
     <row r="7">
@@ -580,16 +580,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.7957164589409468</v>
+        <v>0.8045213424983151</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7804162539177379</v>
+        <v>0.7636442298603677</v>
       </c>
       <c r="E7" t="n">
-        <v>0.7969604299879529</v>
+        <v>0.7972384394402743</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7872969362904352</v>
+        <v>0.7817481003397651</v>
       </c>
     </row>
     <row r="8">
@@ -602,16 +602,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.7879161065596556</v>
+        <v>0.7717053046795664</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7512293710654735</v>
+        <v>0.7320382797320696</v>
       </c>
       <c r="E8" t="n">
-        <v>0.7833379668242053</v>
+        <v>0.7740709850801594</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7670381257688823</v>
+        <v>0.7494307527014981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>